<commit_message>
added PDF for pointcloud polygone creation
</commit_message>
<xml_diff>
--- a/TimeReport-SW-FY190-RB Kruse.xlsx
+++ b/TimeReport-SW-FY190-RB Kruse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Desktop/Research/Dr. Bethel/ROSResearch2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{664F7E8D-ECC1-954A-B0F9-04731F524D09}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64FC3432-44D2-3243-93DA-DBF3F82E33B0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" firstSheet="11" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18088,8 +18088,8 @@
   <dimension ref="A1:L53"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <pane ySplit="13" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
+      <pane ySplit="13" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -18732,7 +18732,7 @@
         <v>19</v>
       </c>
       <c r="C28" s="138">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="D28" s="139"/>
       <c r="E28" s="131"/>
@@ -18760,7 +18760,7 @@
       <c r="B29" s="141"/>
       <c r="C29" s="142">
         <f>SUM(C22:C28)</f>
-        <v>9.5</v>
+        <v>10</v>
       </c>
       <c r="D29" s="142">
         <f>IF(C29&gt;40,C29-40,0)</f>
@@ -18792,7 +18792,9 @@
       <c r="B30" s="144" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="133"/>
+      <c r="C30" s="133">
+        <v>1</v>
+      </c>
       <c r="D30" s="130"/>
       <c r="E30" s="30"/>
       <c r="F30" s="15" t="s">
@@ -18801,7 +18803,7 @@
       <c r="G30" s="29"/>
       <c r="H30" s="31">
         <f>(C21+C29+C37+H21+H29)-C13</f>
-        <v>11</v>
+        <v>12.5</v>
       </c>
       <c r="I30" s="31">
         <f>D21+D29+D37+I21+I29</f>
@@ -18962,7 +18964,7 @@
       <c r="B37" s="149"/>
       <c r="C37" s="142">
         <f>SUM(C30:C36)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D37" s="142">
         <f>IF(C37&gt;40,C37-40,0)</f>
@@ -19624,7 +19626,7 @@
       <c r="B13" s="209"/>
       <c r="C13" s="154">
         <f>'Jan 23, 2020 - Feb 5, 2020'!$C$37</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="154"/>
       <c r="E13" s="155"/>
@@ -19839,7 +19841,7 @@
       <c r="B21" s="141"/>
       <c r="C21" s="142">
         <f>SUM(C13:C20)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="142">
         <f>IF(C21&gt;40,C21-40,0)</f>

</xml_diff>